<commit_message>
Adding required DB fields for collectors
</commit_message>
<xml_diff>
--- a/public/tasks/JHSG_Play_Application_Tasks.xlsx
+++ b/public/tasks/JHSG_Play_Application_Tasks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="-13500" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="5500" yWindow="500" windowWidth="25520" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>JHSG Scala</t>
   </si>
@@ -102,6 +102,14 @@
   </si>
   <si>
     <t>In-progress</t>
+  </si>
+  <si>
+    <t>Update list.scala.html to pull new row
+Update domain.scala to collect status data
+Update form to include status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add validation to Active </t>
   </si>
 </sst>
 </file>
@@ -137,8 +145,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,12 +430,13 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="45" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -509,17 +521,23 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>